<commit_message>
Expand gitignore, wirte README.md and add report
</commit_message>
<xml_diff>
--- a/results/kemerer/weka/test-data-mmre.xlsx
+++ b/results/kemerer/weka/test-data-mmre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mandriv/Documents/final-year-classes/python-projects/cost-estimation/results/kemerer/weka/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74CD627-A44A-EC43-A25E-0CD144C6B38F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C155A04D-139F-BE4D-9508-DD1ADE5301B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5440" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{6929C8CA-2FBA-0E41-8C47-9D3775CA01D7}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="test_data_predictions_1" localSheetId="0">Sheet1!$A$1:$D$6</definedName>
+    <definedName name="test_data_predictions" localSheetId="0">Sheet1!$A$1:$D$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{1457DDCC-8C09-DF4E-8EF7-6AD9DF5C4ABA}" name="test-data-predictions" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{F708CAE0-97EA-AB45-B1F4-2143CE748371}" name="test-data-predictions" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/mandriv/Documents/final-year-classes/python-projects/cost-estimation/results/kemerer/weka/test-data-predictions.csv" comma="1">
       <textFields count="4">
         <textField/>
@@ -63,10 +63,10 @@
     <t>error</t>
   </si>
   <si>
-    <t>mre</t>
+    <t>mmre</t>
   </si>
   <si>
-    <t>mmre</t>
+    <t>mme</t>
   </si>
 </sst>
 </file>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="test-data-predictions_1" connectionId="1" xr16:uid="{7808FF09-679F-294C-9F22-223007B33A4B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="test-data-predictions" connectionId="1" xr16:uid="{8B5C46FF-CB20-564A-AEC9-60A084D8B22C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -425,7 +425,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,7 +449,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -460,14 +460,14 @@
         <v>230.7</v>
       </c>
       <c r="C2">
-        <v>440.26600000000002</v>
+        <v>318.92200000000003</v>
       </c>
       <c r="D2">
-        <v>209.566</v>
+        <v>88.221999999999994</v>
       </c>
       <c r="E2">
-        <f>ABS(B2-C2)/B2</f>
-        <v>0.90839185088860008</v>
+        <f>ABS(C2-B2)/B2</f>
+        <v>0.38241005635023856</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -478,14 +478,14 @@
         <v>72</v>
       </c>
       <c r="C3">
-        <v>-575.56399999999996</v>
+        <v>-255.19499999999999</v>
       </c>
       <c r="D3">
-        <v>-647.56399999999996</v>
+        <v>-327.19499999999999</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E8" si="0">ABS(B3-C3)/B3</f>
-        <v>8.9939444444444447</v>
+        <f t="shared" ref="E3:E6" si="0">ABS(C3-B3)/B3</f>
+        <v>4.5443749999999996</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -496,14 +496,14 @@
         <v>130.30000000000001</v>
       </c>
       <c r="C4">
-        <v>50.51</v>
+        <v>168.95599999999999</v>
       </c>
       <c r="D4">
-        <v>-79.790000000000006</v>
+        <v>38.655999999999999</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0.61235610130468165</v>
+        <v>0.29666922486569436</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -514,14 +514,14 @@
         <v>336.3</v>
       </c>
       <c r="C5">
-        <v>161.749</v>
+        <v>326.00299999999999</v>
       </c>
       <c r="D5">
-        <v>-174.55099999999999</v>
+        <v>-10.297000000000001</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0.51903360095153139</v>
+        <v>3.0618495391019997E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -532,23 +532,23 @@
         <v>287</v>
       </c>
       <c r="C6">
-        <v>466.89400000000001</v>
+        <v>190.108</v>
       </c>
       <c r="D6">
-        <v>179.89400000000001</v>
+        <v>-96.891999999999996</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0.62680836236933801</v>
+        <v>0.33760278745644595</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <f>AVERAGE(E2:E6)</f>
-        <v>2.3321068719917193</v>
+        <v>1.1183351128126797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>